<commit_message>
Bug fixed. Updated user manual.
</commit_message>
<xml_diff>
--- a/test_files/QuestionBank-Template-V2.xlsx
+++ b/test_files/QuestionBank-Template-V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB46126-D327-4FD8-AC38-E0FFF004DF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48970B24-30FB-469E-8716-8D0D7188EBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="224">
   <si>
     <t>T</t>
   </si>
@@ -704,6 +704,15 @@
   </si>
   <si>
     <t>4.png</t>
+  </si>
+  <si>
+    <t>How many corners are there in square?</t>
+  </si>
+  <si>
+    <t>square.png</t>
+  </si>
+  <si>
+    <t>maths</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1125,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45903</v>
+        <v>45923</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1349,16 +1358,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3C1A04-8C9A-4AB3-92D4-9CFE7C63CA0B}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="66.44140625" customWidth="1"/>
     <col min="2" max="6" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1852,6 +1862,35 @@
       </c>
       <c r="I17" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>222</v>
+      </c>
+      <c r="I18" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2604,7 +2643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15F7917-4FC8-4FF7-B762-EA8CF8ABB661}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
QuestionBankTemplateV2 Updated with more questions
</commit_message>
<xml_diff>
--- a/test_files/QuestionBank-Template-V2.xlsx
+++ b/test_files/QuestionBank-Template-V2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AU\3rd-Year_2nd-Sem\CSX3010-SP1\SeniorProject1\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Assumption University\Senior Project 1\SeniorProject1\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48970B24-30FB-469E-8716-8D0D7188EBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1571BC0F-09A1-4F70-8083-EB589E8564CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{EFFFEAF5-3877-4B94-88A7-1185D1104C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="341">
   <si>
     <t>T</t>
   </si>
@@ -713,6 +713,357 @@
   </si>
   <si>
     <t>maths</t>
+  </si>
+  <si>
+    <t>Wich of the follwing is a fruit?</t>
+  </si>
+  <si>
+    <t>Applesss</t>
+  </si>
+  <si>
+    <t>None of the aboves</t>
+  </si>
+  <si>
+    <t>fruit.png</t>
+  </si>
+  <si>
+    <t>What animal do bark?</t>
+  </si>
+  <si>
+    <t>dog.png</t>
+  </si>
+  <si>
+    <t>Where is Eiffel Towerr?</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>tower.png</t>
+  </si>
+  <si>
+    <t>Which is the worssst fruit ever?</t>
+  </si>
+  <si>
+    <t>Grape</t>
+  </si>
+  <si>
+    <t>Appless</t>
+  </si>
+  <si>
+    <t>durian.png</t>
+  </si>
+  <si>
+    <t>Which of this is a public park?</t>
+  </si>
+  <si>
+    <t>Greenfeild</t>
+  </si>
+  <si>
+    <t>City Librry</t>
+  </si>
+  <si>
+    <t>Parksss</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Train Stashion</t>
+  </si>
+  <si>
+    <t>Theaterss</t>
+  </si>
+  <si>
+    <t>park2.png</t>
+  </si>
+  <si>
+    <t>How many corners has a squar?</t>
+  </si>
+  <si>
+    <t>square2.png</t>
+  </si>
+  <si>
+    <t>How many corner are in a square?</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>square3.png</t>
+  </si>
+  <si>
+    <t>Which of the follwing is an animall?</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>anim1.png</t>
+  </si>
+  <si>
+    <t>Wich is your favorit place?</t>
+  </si>
+  <si>
+    <t>Parkk</t>
+  </si>
+  <si>
+    <t>Homess</t>
+  </si>
+  <si>
+    <t>Malll</t>
+  </si>
+  <si>
+    <t>Pooll</t>
+  </si>
+  <si>
+    <t>Theatersss</t>
+  </si>
+  <si>
+    <t>place1.png</t>
+  </si>
+  <si>
+    <t>What animal can flying?</t>
+  </si>
+  <si>
+    <t>bird2.png</t>
+  </si>
+  <si>
+    <t>What is the badest fruit?</t>
+  </si>
+  <si>
+    <t>Applle</t>
+  </si>
+  <si>
+    <t>Potato</t>
+  </si>
+  <si>
+    <t>fruit2.png</t>
+  </si>
+  <si>
+    <t>Wich of the follwing is a beeverage?</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Juicc</t>
+  </si>
+  <si>
+    <t>drink1.png</t>
+  </si>
+  <si>
+    <t>bird3.png</t>
+  </si>
+  <si>
+    <t>Which animal can flyy?</t>
+  </si>
+  <si>
+    <t>bird4.png</t>
+  </si>
+  <si>
+    <t>How many corner does a square has?</t>
+  </si>
+  <si>
+    <t>square4.png</t>
+  </si>
+  <si>
+    <t>How many cornes in square?</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>square5.png</t>
+  </si>
+  <si>
+    <t>Where is Chaoo Phara River?</t>
+  </si>
+  <si>
+    <t>river2.png</t>
+  </si>
+  <si>
+    <t>Something soft.</t>
+  </si>
+  <si>
+    <t>5.png</t>
+  </si>
+  <si>
+    <t>Something crunchy.</t>
+  </si>
+  <si>
+    <t>Chips</t>
+  </si>
+  <si>
+    <t>Something hot.</t>
+  </si>
+  <si>
+    <t>Something cold.</t>
+  </si>
+  <si>
+    <t>Something green.</t>
+  </si>
+  <si>
+    <t>Spinach</t>
+  </si>
+  <si>
+    <t>vegetables</t>
+  </si>
+  <si>
+    <t>6.png</t>
+  </si>
+  <si>
+    <t>Something red.</t>
+  </si>
+  <si>
+    <t>Tomato</t>
+  </si>
+  <si>
+    <t>Something yellow.</t>
+  </si>
+  <si>
+    <t>fruit</t>
+  </si>
+  <si>
+    <t>7.png</t>
+  </si>
+  <si>
+    <t>Something purple.</t>
+  </si>
+  <si>
+    <t>Something round.</t>
+  </si>
+  <si>
+    <t>Ball</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>8.png</t>
+  </si>
+  <si>
+    <t>Something square.</t>
+  </si>
+  <si>
+    <t>Dice</t>
+  </si>
+  <si>
+    <t>Something that fly.</t>
+  </si>
+  <si>
+    <t>9.png</t>
+  </si>
+  <si>
+    <t>Something that swim.</t>
+  </si>
+  <si>
+    <t>Something that bark.</t>
+  </si>
+  <si>
+    <t>10.png</t>
+  </si>
+  <si>
+    <t>Something that meow.</t>
+  </si>
+  <si>
+    <t>Something used to write.</t>
+  </si>
+  <si>
+    <t>Pen</t>
+  </si>
+  <si>
+    <t>11.png</t>
+  </si>
+  <si>
+    <t>Something used to cut.</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Something used to eat soup.</t>
+  </si>
+  <si>
+    <t>Spoon</t>
+  </si>
+  <si>
+    <t>utensil</t>
+  </si>
+  <si>
+    <t>12.png</t>
+  </si>
+  <si>
+    <t>Something used to eat rice.</t>
+  </si>
+  <si>
+    <t>Fork</t>
+  </si>
+  <si>
+    <t>Something you wear on foot.</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>clothing</t>
+  </si>
+  <si>
+    <t>13.png</t>
+  </si>
+  <si>
+    <t>Something you wear on head.</t>
+  </si>
+  <si>
+    <t>Hat</t>
+  </si>
+  <si>
+    <t>Something that shine at night.</t>
+  </si>
+  <si>
+    <t>Moon</t>
+  </si>
+  <si>
+    <t>nature</t>
+  </si>
+  <si>
+    <t>14.png</t>
+  </si>
+  <si>
+    <t>Something that shine at day.</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Something we drink in morning.</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>drink</t>
+  </si>
+  <si>
+    <t>15.png</t>
+  </si>
+  <si>
+    <t>Something we drink when hot.</t>
   </si>
 </sst>
 </file>
@@ -754,7 +1105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -765,6 +1116,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1125,7 +1479,7 @@
       </c>
       <c r="Q1" s="3">
         <f ca="1">TODAY()</f>
-        <v>45923</v>
+        <v>45926</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1358,17 +1712,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA3C1A04-8C9A-4AB3-92D4-9CFE7C63CA0B}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="66.44140625" customWidth="1"/>
     <col min="2" max="6" width="15.77734375" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1891,6 +2245,528 @@
       </c>
       <c r="I18" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>2</v>
+      </c>
+      <c r="D25" s="6">
+        <v>3</v>
+      </c>
+      <c r="E25" s="6">
+        <v>4</v>
+      </c>
+      <c r="F25" s="6">
+        <v>5</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B34" s="6">
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
+        <v>2</v>
+      </c>
+      <c r="D34" s="6">
+        <v>3</v>
+      </c>
+      <c r="E34" s="6">
+        <v>4</v>
+      </c>
+      <c r="F34" s="6">
+        <v>6</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1903,7 +2779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589423D0-50CB-4F3F-82F4-CB353E932D78}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
@@ -2495,10 +3371,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFE4AC3-D33B-41F7-AFE1-650B291E6FA6}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2634,6 +3510,342 @@
         <v>218</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2644,7 +3856,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>